<commit_message>
0 validations fpor paclages
</commit_message>
<xml_diff>
--- a/src/PeStopAnnualReport/PSARTests/Data/invalid_package_year_sheet.xlsx
+++ b/src/PeStopAnnualReport/PSARTests/Data/invalid_package_year_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eu\GitHub\PeStop\src\PeStopAnnualReport\PSARTests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77237DC7-E28F-4EC1-A566-61052416EA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8098DA93-4BC8-4268-8E11-AD494EB542AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>